<commit_message>
Clean up workspace: remove backup files, temporary files, and unnecessary files
</commit_message>
<xml_diff>
--- a/PriceLists/productData.xlsx
+++ b/PriceLists/productData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inh\inh\PriceLists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D94786-4AC7-437B-9890-592AA6980AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5723BD7-7168-4510-BC33-DD5E8C2312B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB16E37F-FFE5-450C-AB63-D48333F2CE3E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AB16E37F-FFE5-450C-AB63-D48333F2CE3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="salesmen" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$621</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4350" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4358" uniqueCount="93">
   <si>
     <t>Length</t>
   </si>
@@ -294,6 +295,30 @@
   </si>
   <si>
     <t>Genius</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Praveen</t>
+  </si>
+  <si>
+    <t>Rupa</t>
+  </si>
+  <si>
+    <t>INH</t>
+  </si>
+  <si>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>Vijay</t>
+  </si>
+  <si>
+    <t>Pankaj</t>
+  </si>
+  <si>
+    <t>Sunil</t>
   </si>
 </sst>
 </file>
@@ -795,7 +820,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J621"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D281" sqref="D281:D290"/>
     </sheetView>
   </sheetViews>
@@ -20694,4 +20719,59 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DB8141-BC1D-4A77-8FB1-1D5D8A34A002}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>